<commit_message>
a version with all figures
</commit_message>
<xml_diff>
--- a/app/static/Flu09/all_results.xlsx
+++ b/app/static/Flu09/all_results.xlsx
@@ -241,7 +241,7 @@
     <t>clustering_abs</t>
   </si>
   <si>
-    <t>correlation_figures_Flu09_Plasma_absolute_</t>
+    <t>correlation_abs</t>
   </si>
   <si>
     <t>outcome_abs</t>
@@ -250,7 +250,7 @@
     <t>clustering_adj</t>
   </si>
   <si>
-    <t>correlation_figures_Flu09_Plasma_adjusted_</t>
+    <t>correlation_adj</t>
   </si>
   <si>
     <t>outcome_adj</t>

</xml_diff>